<commit_message>
Added more unit tests
</commit_message>
<xml_diff>
--- a/unit_test/dataframes/happy/df_1.xlsx
+++ b/unit_test/dataframes/happy/df_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -72,6 +72,57 @@
   </si>
   <si>
     <t xml:space="preserve">Heal, Mana, PayLife, Ability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regrowth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fuel -- return target card from your discard to your hand.
+Choose two (</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">you can choose each mode multiple times</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">):
+ - return target card from any discard to it's owner's hand;
+ - remove target card from any discard.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://c4.wallpaperflare.com/wallpaper/773/817/71/green-light-sake-girl-wallpaper-preview.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel, Recursion, Gravehate</t>
   </si>
 </sst>
 </file>
@@ -81,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,6 +174,14 @@
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -293,10 +352,10 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="3:7"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.99"/>
   </cols>
@@ -371,18 +430,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="1"/>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -517,6 +598,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://99px.ru/sstorage/56/2013/06/10306130220478230.jpg"/>
+    <hyperlink ref="I3" r:id="rId2" display="https://c4.wallpaperflare.com/wallpaper/773/817/71/green-light-sake-girl-wallpaper-preview.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>